<commit_message>
Universal Calculator with RUB calculated correctly
</commit_message>
<xml_diff>
--- a/src/RUB_Inflation.xlsx
+++ b/src/RUB_Inflation.xlsx
@@ -2,91 +2,55 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11210"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sveta/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sveta/Svetas_project/time_convert_app/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D5FABB0-999C-8442-B546-FEA3D6132221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D44409AF-5D75-484B-8D8E-B26FF58F62B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="500" windowWidth="18200" windowHeight="8500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="01" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>inflation</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="_-* #,##0\ &quot;₽&quot;_-;\-* #,##0\ &quot;₽&quot;_-;_-* &quot;-&quot;\ &quot;₽&quot;_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0\ _₽_-;\-* #,##0\ _₽_-;_-* &quot;-&quot;\ _₽_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0.00\ &quot;₽&quot;_-;\-* #,##0.00\ &quot;₽&quot;_-;_-* &quot;-&quot;??\ &quot;₽&quot;_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
-  </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -98,7 +62,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -108,86 +72,65 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="20">
-    <cellStyle name="Comma" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Comma [0]" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Currency" xfId="4" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Currency [0]" xfId="5" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Обычный 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Обычный 2 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="Обычный 2 2 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="Обычный 2 3" xfId="9" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="Обычный 3" xfId="10" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="Обычный 3 2" xfId="11" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="Обычный 3 2 2" xfId="12" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
-    <cellStyle name="Обычный 3 3" xfId="13" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
-    <cellStyle name="Обычный 4" xfId="14" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
-    <cellStyle name="Обычный 5" xfId="15" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
-    <cellStyle name="Обычный 5 2" xfId="16" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="Обычный 6" xfId="17" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
-    <cellStyle name="Обычный 7" xfId="18" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
-    <cellStyle name="Обычный 8" xfId="19" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -200,9 +143,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -240,7 +183,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -312,7 +255,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -333,7 +276,6 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
@@ -344,31 +286,31 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
+                <a:tint val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
+                <a:tint val="15000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
+                <a:tint val="94000"/>
                 <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
+              <a:shade val="9500"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
@@ -390,7 +332,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -448,7 +390,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
+                <a:tint val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -461,13 +403,12 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
                 <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -485,297 +426,293 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
+    <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" style="1" customWidth="1"/>
-    <col min="6" max="24" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6" style="1" customWidth="1"/>
-    <col min="26" max="27" width="7.33203125" style="1" customWidth="1"/>
-    <col min="28" max="30" width="7.1640625" style="1" customWidth="1"/>
-    <col min="31" max="33" width="6.6640625" style="1" customWidth="1"/>
-    <col min="34" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="9.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="3">
+    <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
         <v>1991</v>
       </c>
-      <c r="B1" s="2">
+      <c r="B2" s="3">
         <v>160.39999999999998</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
+    <row r="3" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
         <v>1992</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B3" s="3">
         <v>2508.84</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
+    <row r="4" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
         <v>1993</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B4" s="3">
         <v>839.9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
+    <row r="5" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
         <v>1994</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B5" s="3">
         <v>215.14</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
+    <row r="6" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>1995</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B6" s="3">
         <v>131.30000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
+    <row r="7" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
         <v>1996</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B7" s="3">
         <v>21.810000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
+    <row r="8" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
         <v>1997</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B8" s="3">
         <v>11.030000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
+    <row r="9" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
         <v>1998</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B9" s="3">
         <v>84.43</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
+    <row r="10" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
         <v>1999</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B10" s="3">
         <v>36.53</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
+    <row r="11" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
         <v>2000</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B11" s="3">
         <v>20.180000000000007</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
+    <row r="12" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
         <v>2001</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B12" s="3">
         <v>18.579999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
+    <row r="13" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
         <v>2002</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B13" s="3">
         <v>15.060000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
+    <row r="14" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
         <v>2003</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B14" s="3">
         <v>11.989999999999995</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
+    <row r="15" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
         <v>2004</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B15" s="3">
         <v>11.730000000000004</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
+    <row r="16" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
         <v>2005</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B16" s="3">
         <v>10.920000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="3">
+    <row r="17" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
         <v>2006</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B17" s="3">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="3">
+    <row r="18" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
         <v>2007</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B18" s="3">
         <v>11.870000000000005</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="3">
+    <row r="19" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
         <v>2008</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B19" s="3">
         <v>13.280000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="3">
+    <row r="20" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
         <v>2009</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B20" s="3">
         <v>8.7999999999999972</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="3">
+    <row r="21" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
         <v>2010</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B21" s="3">
         <v>8.7800000000000011</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="3">
+    <row r="22" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
         <v>2011</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B22" s="3">
         <v>6.0999999999999943</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="3">
+    <row r="23" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
         <v>2012</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B23" s="3">
         <v>6.5699999999999932</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="4">
+    <row r="24" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="4">
         <v>2013</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B24" s="3">
         <v>6.4699999999999989</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="4">
+    <row r="25" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="4">
         <v>2014</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B25" s="3">
         <v>11.349999999999994</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="3">
+    <row r="26" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
         <v>2015</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B26" s="3">
         <v>12.909999999999997</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="3">
+    <row r="27" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
         <v>2016</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B27" s="3">
         <v>5.3900000000000006</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="3">
+    <row r="28" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
         <v>2017</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B28" s="3">
         <v>2.5100000000000051</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="3">
+    <row r="29" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
         <v>2018</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B29" s="3">
         <v>4.2600000000000051</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="3">
+    <row r="30" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
         <v>2019</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B30" s="3">
         <v>3.0400000000000063</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="3">
+    <row r="31" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
         <v>2020</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B31" s="3">
         <v>4.9099999999999966</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="3">
+    <row r="32" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
         <v>2021</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B32" s="3">
         <v>8.39</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="3">
+    <row r="33" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
         <v>2022</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B33" s="3">
         <v>11.939999999999998</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="3">
+    <row r="34" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
         <v>2023</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B34" s="3">
         <v>7.4200000000000017</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.21" right="0.19685039370078741" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="81" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Started working with USD-inflation. WIP
</commit_message>
<xml_diff>
--- a/src/RUB_Inflation.xlsx
+++ b/src/RUB_Inflation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sveta/Svetas_project/time_convert_app/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D44409AF-5D75-484B-8D8E-B26FF58F62B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1EADD4-1347-3048-90CC-B3A5EC5BF378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="500" windowWidth="18200" windowHeight="8500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -432,7 +432,9 @@
   </sheetPr>
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>